<commit_message>
Added totals, chronological order, fixed AllPlaylist...
</commit_message>
<xml_diff>
--- a/CheckList_Final.xlsx
+++ b/CheckList_Final.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Werk\220\2024\Project\D3 (Final)\Marking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knock\OneDrive\Documents\UP\#Semester 2\IMY220\Project\IMY220_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEE7C93-402B-436D-B3A7-D99D724B465E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF60098-3420-4475-8053-A85EEDC43987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9sub6SWNHua8xXmx+dlzyISY4/kLd62l4tl3wjOTM1s="/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="165">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -713,6 +724,12 @@
   </si>
   <si>
     <t>Can build and run project using Docker CLI</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -962,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1001,6 +1018,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1220,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1416,28 +1436,36 @@
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="33"/>
+      <c r="B38" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C38" s="11"/>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="33"/>
+      <c r="B39" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="33"/>
+      <c r="B40" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C40" s="11"/>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="33"/>
+      <c r="B41" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1450,84 +1478,108 @@
       <c r="A44" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="33"/>
+      <c r="B44" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="33"/>
+      <c r="B46" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C46" s="11"/>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="33"/>
+      <c r="B47" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="33"/>
+      <c r="B48" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="33"/>
+      <c r="B49" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C49" s="11"/>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="33"/>
+      <c r="B50" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C50" s="11"/>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="33"/>
+      <c r="B51" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C51" s="11"/>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="33"/>
+      <c r="B52" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C53" s="11"/>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="33"/>
+      <c r="B54" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C54" s="11"/>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="33"/>
+      <c r="B55" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C55" s="11"/>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1552,35 +1604,45 @@
       <c r="A60" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="33"/>
+      <c r="B60" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C60" s="11"/>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B61" s="33"/>
+      <c r="B61" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C61" s="11"/>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="33"/>
+      <c r="B62" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C62" s="11"/>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="33"/>
+      <c r="B63" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C63" s="11"/>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B64" s="33"/>
+      <c r="B64" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C64" s="11"/>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1602,38 +1664,48 @@
       <c r="A68" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="33"/>
+      <c r="B68" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="33"/>
+      <c r="B69" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C69" s="11"/>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B70" s="33"/>
+      <c r="B70" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="33"/>
+      <c r="B71" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C71" s="11"/>
     </row>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="33"/>
+      <c r="B72" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C72" s="11"/>
     </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>61</v>
       </c>
@@ -1644,7 +1716,7 @@
       <c r="A74" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B74" s="33"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="11"/>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1657,14 +1729,18 @@
       <c r="A77" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B77" s="33"/>
+      <c r="B77" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C77" s="11"/>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="33"/>
+      <c r="B78" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C78" s="11"/>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1678,7 +1754,9 @@
       <c r="A80" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B80" s="33"/>
+      <c r="B80" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C80" s="11"/>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1706,7 +1784,9 @@
       <c r="A84" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B84" s="33"/>
+      <c r="B84" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C84" s="11"/>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1724,14 +1804,18 @@
       <c r="A88" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="33"/>
+      <c r="B88" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C88" s="11"/>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B89" s="33"/>
+      <c r="B89" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C89" s="11"/>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1774,7 +1858,9 @@
       <c r="A95" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="33"/>
+      <c r="B95" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C95" s="11"/>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1802,7 +1888,9 @@
       <c r="A99" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B99" s="33"/>
+      <c r="B99" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C99" s="11"/>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1816,7 +1904,9 @@
       <c r="A101" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="33"/>
+      <c r="B101" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C101" s="11"/>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1853,42 +1943,54 @@
       <c r="A107" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B107" s="33"/>
+      <c r="B107" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C107" s="11"/>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B108" s="33"/>
+      <c r="B108" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C108" s="11"/>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B109" s="33"/>
+      <c r="B109" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C109" s="11"/>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B110" s="33"/>
+      <c r="B110" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C110" s="11"/>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B111" s="33"/>
+      <c r="B111" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C111" s="11"/>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B112" s="33"/>
+      <c r="B112" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C112" s="11"/>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1920,14 +2022,18 @@
       <c r="A117" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B117" s="33"/>
+      <c r="B117" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C117" s="11"/>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B118" s="33"/>
+      <c r="B118" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C118" s="11"/>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1941,7 +2047,9 @@
       <c r="A120" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B120" s="33"/>
+      <c r="B120" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C120" s="11"/>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,7 +2063,9 @@
       <c r="A122" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B122" s="33"/>
+      <c r="B122" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C122" s="11"/>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2177,14 +2287,18 @@
       <c r="A151" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B151" s="33"/>
+      <c r="B151" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C151" s="11"/>
     </row>
     <row r="152" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B152" s="33"/>
+      <c r="B152" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C152" s="11"/>
     </row>
     <row r="153" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2209,21 +2323,27 @@
       <c r="A156" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B156" s="33"/>
+      <c r="B156" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C156" s="11"/>
     </row>
     <row r="157" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B157" s="33"/>
+      <c r="B157" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C157" s="11"/>
     </row>
     <row r="158" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B158" s="33"/>
+      <c r="B158" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C158" s="11"/>
     </row>
     <row r="159" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2237,21 +2357,27 @@
       <c r="A160" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B160" s="33"/>
+      <c r="B160" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C160" s="11"/>
     </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B161" s="33"/>
+      <c r="B161" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C161" s="11"/>
     </row>
     <row r="162" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B162" s="33"/>
+      <c r="B162" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C162" s="11"/>
     </row>
     <row r="163" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2265,7 +2391,9 @@
       <c r="A164" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B164" s="33"/>
+      <c r="B164" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C164" s="11"/>
     </row>
     <row r="165" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,28 +2457,36 @@
       <c r="A174" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B174" s="33"/>
+      <c r="B174" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C174" s="11"/>
     </row>
     <row r="175" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B175" s="33"/>
+      <c r="B175" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C175" s="11"/>
     </row>
     <row r="176" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B176" s="33"/>
+      <c r="B176" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C176" s="11"/>
     </row>
     <row r="177" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B177" s="33"/>
+      <c r="B177" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C177" s="11"/>
     </row>
     <row r="178" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2375,21 +2511,27 @@
       <c r="A181" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B181" s="33"/>
+      <c r="B181" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C181" s="11"/>
     </row>
     <row r="182" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B182" s="33"/>
+      <c r="B182" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C182" s="11"/>
     </row>
     <row r="183" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B183" s="33"/>
+      <c r="B183" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C183" s="11"/>
       <c r="D183" s="13"/>
     </row>
@@ -2397,7 +2539,9 @@
       <c r="A184" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B184" s="33"/>
+      <c r="B184" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C184" s="11"/>
       <c r="D184" s="13"/>
     </row>
@@ -2405,7 +2549,9 @@
       <c r="A185" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B185" s="33"/>
+      <c r="B185" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C185" s="11"/>
       <c r="D185" s="13"/>
     </row>
@@ -2413,35 +2559,45 @@
       <c r="A186" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B186" s="33"/>
+      <c r="B186" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C186" s="11"/>
     </row>
     <row r="187" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B187" s="33"/>
+      <c r="B187" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C187" s="11"/>
     </row>
     <row r="188" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B188" s="33"/>
+      <c r="B188" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C188" s="11"/>
     </row>
     <row r="189" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="B189" s="33"/>
+      <c r="B189" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C189" s="11"/>
     </row>
     <row r="190" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B190" s="33"/>
+      <c r="B190" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C190" s="11"/>
     </row>
     <row r="191" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added song page and changed the searching functionality
</commit_message>
<xml_diff>
--- a/CheckList_Final.xlsx
+++ b/CheckList_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knock\OneDrive\Documents\UP\#Semester 2\IMY220\Project\IMY220_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF60098-3420-4475-8053-A85EEDC43987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E43A62-704F-4760-A11B-F5C88154A712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="166">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -730,6 +730,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1240,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1586,7 +1589,9 @@
       <c r="A56" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="33"/>
+      <c r="B56" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C56" s="11"/>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1836,7 +1841,9 @@
       <c r="A92" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B92" s="33"/>
+      <c r="B92" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C92" s="11"/>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1897,7 +1904,9 @@
       <c r="A100" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B100" s="33"/>
+      <c r="B100" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C100" s="11"/>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1905,7 +1914,7 @@
         <v>85</v>
       </c>
       <c r="B101" s="33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C101" s="11"/>
     </row>
@@ -1997,14 +2006,18 @@
       <c r="A113" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="33"/>
+      <c r="B113" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C113" s="11"/>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B114" s="33"/>
+      <c r="B114" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C114" s="11"/>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final changes before submission
</commit_message>
<xml_diff>
--- a/CheckList_Final.xlsx
+++ b/CheckList_Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knock\OneDrive\Documents\UP\#Semester 2\IMY220\Project\IMY220_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knock\OneDrive\Documents\UP\Semester 2\IMY220\Project\IMY220_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E43A62-704F-4760-A11B-F5C88154A712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176635F0-75D2-450F-A882-4756F9FD686A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="1980" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="166">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1714,7 +1714,9 @@
       <c r="A73" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="33"/>
+      <c r="B73" s="33" t="s">
+        <v>163</v>
+      </c>
       <c r="C73" s="11"/>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>